<commit_message>
Redigert etter ønske fra kunde
</commit_message>
<xml_diff>
--- a/Sprint 4/SysUt14 Gr 2 Burn up chart - holdes oppdatert.xlsx
+++ b/Sprint 4/SysUt14 Gr 2 Burn up chart - holdes oppdatert.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -11,12 +11,12 @@
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Start</t>
   </si>
@@ -199,13 +199,25 @@
   </si>
   <si>
     <t>Opprette milepæler i prosjekt</t>
+  </si>
+  <si>
+    <t>Dokumentasjon</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Planlegging av prosjekt, programmering, osv.</t>
+  </si>
+  <si>
+    <t>Testing av alle typer kode.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -349,12 +361,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -418,6 +441,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -444,19 +470,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="nb-NO"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -471,7 +486,6 @@
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -483,59 +497,58 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$E$16:$S$16</c:f>
+              <c:f>'Ark1'!$E$20:$S$20</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>-4.2632564145606011E-14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.857142857142815</c:v>
+                  <c:v>36.444444444444443</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.714285714285673</c:v>
+                  <c:v>36.444444444444443</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.57142857142853</c:v>
+                  <c:v>63.777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.428571428571388</c:v>
+                  <c:v>63.777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44.285714285714249</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53.14285714285711</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>61.999999999999972</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70.857142857142833</c:v>
+                  <c:v>109.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>79.714285714285694</c:v>
+                  <c:v>109.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.571428571428555</c:v>
+                  <c:v>136.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>97.428571428571416</c:v>
+                  <c:v>136.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>106.28571428571428</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>115.14285714285714</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>124</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -548,105 +561,56 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$E$17:$S$17</c:f>
+              <c:f>'Ark1'!$E$21:$S$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>6.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="46504960"/>
-        <c:axId val="46527232"/>
+        <c:axId val="101371264"/>
+        <c:axId val="101377152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46504960"/>
+        <c:axId val="101371264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46527232"/>
+        <c:crossAx val="101377152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46527232"/>
+        <c:axId val="101377152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
           <c:min val="0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46504960"/>
+        <c:crossAx val="101371264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -657,13 +621,12 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.85726259133462968"/>
+          <c:x val="0.85726259133462956"/>
           <c:y val="0.42329864488726682"/>
           <c:w val="0.1364510697882074"/>
-          <c:h val="0.15646062275472189"/>
+          <c:h val="0.15646062275472192"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -677,7 +640,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -694,13 +656,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>197938</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>104384</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>147440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -841,7 +803,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -876,7 +837,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1052,17 +1012,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
@@ -1071,7 +1031,7 @@
     <col min="5" max="19" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15.75">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1130,7 +1090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
@@ -1144,52 +1104,30 @@
         <v>5</v>
       </c>
       <c r="E2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H2" s="8">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8">
-        <v>0</v>
-      </c>
-      <c r="J2" s="8">
-        <v>0</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0</v>
-      </c>
-      <c r="L2" s="8">
-        <v>0</v>
-      </c>
-      <c r="M2" s="8">
-        <v>0</v>
-      </c>
-      <c r="N2" s="8">
-        <v>0</v>
-      </c>
-      <c r="O2" s="8">
-        <v>0</v>
-      </c>
-      <c r="P2" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>0</v>
-      </c>
-      <c r="R2" s="8">
-        <v>0</v>
-      </c>
-      <c r="S2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -1214,41 +1152,18 @@
       <c r="H3" s="8">
         <v>0</v>
       </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="8">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>0</v>
-      </c>
-      <c r="R3" s="8">
-        <v>0</v>
-      </c>
-      <c r="S3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1261,7 +1176,7 @@
       <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <v>0</v>
       </c>
       <c r="F4" s="10">
@@ -1273,41 +1188,19 @@
       <c r="H4" s="10">
         <v>0</v>
       </c>
-      <c r="I4" s="10">
-        <v>0</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0</v>
-      </c>
-      <c r="M4" s="10">
-        <v>0</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0</v>
-      </c>
-      <c r="O4" s="10">
-        <v>0</v>
-      </c>
-      <c r="P4" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>0</v>
-      </c>
-      <c r="R4" s="8">
-        <v>0</v>
-      </c>
-      <c r="S4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75">
       <c r="A5" s="6" t="s">
         <v>58</v>
       </c>
@@ -1320,53 +1213,31 @@
       <c r="D5" s="10">
         <v>4</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>0</v>
       </c>
       <c r="F5" s="10">
         <v>2</v>
       </c>
       <c r="G5" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" s="10">
-        <v>0</v>
-      </c>
-      <c r="I5" s="10">
-        <v>0</v>
-      </c>
-      <c r="J5" s="10">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0</v>
-      </c>
-      <c r="L5" s="10">
-        <v>0</v>
-      </c>
-      <c r="M5" s="10">
-        <v>0</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0</v>
-      </c>
-      <c r="O5" s="10">
-        <v>0</v>
-      </c>
-      <c r="P5" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>0</v>
-      </c>
-      <c r="R5" s="8">
-        <v>0</v>
-      </c>
-      <c r="S5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -1379,8 +1250,8 @@
       <c r="D6" s="10">
         <v>10</v>
       </c>
-      <c r="E6" s="10">
-        <v>5</v>
+      <c r="E6" s="8">
+        <v>0</v>
       </c>
       <c r="F6" s="10">
         <v>0</v>
@@ -1391,41 +1262,19 @@
       <c r="H6" s="10">
         <v>0</v>
       </c>
-      <c r="I6" s="10">
-        <v>0</v>
-      </c>
-      <c r="J6" s="10">
-        <v>0</v>
-      </c>
-      <c r="K6" s="10">
-        <v>0</v>
-      </c>
-      <c r="L6" s="10">
-        <v>0</v>
-      </c>
-      <c r="M6" s="10">
-        <v>0</v>
-      </c>
-      <c r="N6" s="10">
-        <v>0</v>
-      </c>
-      <c r="O6" s="10">
-        <v>0</v>
-      </c>
-      <c r="P6" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>0</v>
-      </c>
-      <c r="R6" s="8">
-        <v>0</v>
-      </c>
-      <c r="S6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75">
       <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
@@ -1438,53 +1287,31 @@
       <c r="D7" s="10">
         <v>1</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>0</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="10">
-        <v>0</v>
-      </c>
-      <c r="I7" s="10">
-        <v>0</v>
-      </c>
-      <c r="J7" s="10">
-        <v>0</v>
-      </c>
-      <c r="K7" s="10">
-        <v>0</v>
-      </c>
-      <c r="L7" s="10">
-        <v>0</v>
-      </c>
-      <c r="M7" s="10">
-        <v>0</v>
-      </c>
-      <c r="N7" s="10">
-        <v>0</v>
-      </c>
-      <c r="O7" s="10">
-        <v>0</v>
-      </c>
-      <c r="P7" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>0</v>
-      </c>
-      <c r="R7" s="8">
-        <v>0</v>
-      </c>
-      <c r="S7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75">
       <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
@@ -1498,52 +1325,30 @@
         <v>2.5</v>
       </c>
       <c r="E8" s="8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F8" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="8">
-        <v>0</v>
-      </c>
-      <c r="M8" s="24">
-        <v>0</v>
-      </c>
-      <c r="N8" s="24">
-        <v>0</v>
-      </c>
-      <c r="O8" s="24">
-        <v>0</v>
-      </c>
-      <c r="P8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>0</v>
-      </c>
-      <c r="R8" s="8">
-        <v>0</v>
-      </c>
-      <c r="S8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75">
       <c r="A9" s="6"/>
       <c r="B9" s="23" t="s">
         <v>32</v>
@@ -1558,49 +1363,27 @@
         <v>0</v>
       </c>
       <c r="F9" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0</v>
-      </c>
-      <c r="K9" s="8">
-        <v>0</v>
-      </c>
-      <c r="L9" s="8">
-        <v>0</v>
-      </c>
-      <c r="M9" s="24">
-        <v>0</v>
-      </c>
-      <c r="N9" s="24">
-        <v>0</v>
-      </c>
-      <c r="O9" s="24">
-        <v>0</v>
-      </c>
-      <c r="P9" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>0</v>
-      </c>
-      <c r="R9" s="8">
-        <v>0</v>
-      </c>
-      <c r="S9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75">
       <c r="A10" s="6" t="s">
         <v>54</v>
       </c>
@@ -1625,41 +1408,19 @@
       <c r="H10" s="8">
         <v>0</v>
       </c>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-      <c r="K10" s="8">
-        <v>0</v>
-      </c>
-      <c r="L10" s="8">
-        <v>0</v>
-      </c>
-      <c r="M10" s="24">
-        <v>0</v>
-      </c>
-      <c r="N10" s="24">
-        <v>0</v>
-      </c>
-      <c r="O10" s="24">
-        <v>0</v>
-      </c>
-      <c r="P10" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>0</v>
-      </c>
-      <c r="R10" s="8">
-        <v>0</v>
-      </c>
-      <c r="S10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75">
       <c r="A11" s="6"/>
       <c r="B11" s="23" t="s">
         <v>45</v>
@@ -1682,41 +1443,19 @@
       <c r="H11" s="8">
         <v>0</v>
       </c>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
-        <v>0</v>
-      </c>
-      <c r="M11" s="24">
-        <v>0</v>
-      </c>
-      <c r="N11" s="24">
-        <v>0</v>
-      </c>
-      <c r="O11" s="24">
-        <v>0</v>
-      </c>
-      <c r="P11" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="8">
-        <v>0</v>
-      </c>
-      <c r="R11" s="8">
-        <v>0</v>
-      </c>
-      <c r="S11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75">
       <c r="A12" s="6"/>
       <c r="B12" s="23" t="s">
         <v>47</v>
@@ -1739,41 +1478,19 @@
       <c r="H12" s="8">
         <v>0</v>
       </c>
-      <c r="I12" s="8">
-        <v>0</v>
-      </c>
-      <c r="J12" s="8">
-        <v>0</v>
-      </c>
-      <c r="K12" s="8">
-        <v>0</v>
-      </c>
-      <c r="L12" s="8">
-        <v>0</v>
-      </c>
-      <c r="M12" s="24">
-        <v>0</v>
-      </c>
-      <c r="N12" s="24">
-        <v>0</v>
-      </c>
-      <c r="O12" s="24">
-        <v>0</v>
-      </c>
-      <c r="P12" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="8">
-        <v>0</v>
-      </c>
-      <c r="R12" s="8">
-        <v>0</v>
-      </c>
-      <c r="S12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75">
       <c r="A13" s="6" t="s">
         <v>53</v>
       </c>
@@ -1798,41 +1515,19 @@
       <c r="H13" s="8">
         <v>0</v>
       </c>
-      <c r="I13" s="8">
-        <v>0</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <v>0</v>
-      </c>
-      <c r="M13" s="24">
-        <v>0</v>
-      </c>
-      <c r="N13" s="24">
-        <v>0</v>
-      </c>
-      <c r="O13" s="24">
-        <v>0</v>
-      </c>
-      <c r="P13" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>0</v>
-      </c>
-      <c r="R13" s="8">
-        <v>0</v>
-      </c>
-      <c r="S13" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75">
       <c r="A14" s="6"/>
       <c r="B14" s="23" t="s">
         <v>51</v>
@@ -1855,264 +1550,306 @@
       <c r="H14" s="8">
         <v>0</v>
       </c>
-      <c r="I14" s="8">
-        <v>0</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0</v>
-      </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>0</v>
-      </c>
-      <c r="M14" s="24">
-        <v>0</v>
-      </c>
-      <c r="N14" s="24">
-        <v>0</v>
-      </c>
-      <c r="O14" s="24">
-        <v>0</v>
-      </c>
-      <c r="P14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>0</v>
-      </c>
-      <c r="R14" s="8">
-        <v>0</v>
-      </c>
-      <c r="S14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75">
+      <c r="A15" s="6"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75">
+      <c r="A16" s="6"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75">
+      <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B17" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D17" s="8">
         <v>40</v>
       </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="8">
-        <v>2</v>
-      </c>
-      <c r="G15" s="8">
-        <v>0</v>
-      </c>
-      <c r="H15" s="8">
-        <v>0</v>
-      </c>
-      <c r="I15" s="8">
-        <v>0</v>
-      </c>
-      <c r="J15" s="8">
-        <v>0</v>
-      </c>
-      <c r="K15" s="8">
-        <v>0</v>
-      </c>
-      <c r="L15" s="8">
-        <v>0</v>
-      </c>
-      <c r="M15" s="8">
-        <v>0</v>
-      </c>
-      <c r="N15" s="8">
-        <v>0</v>
-      </c>
-      <c r="O15" s="8">
-        <v>0</v>
-      </c>
-      <c r="P15" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="8">
-        <v>0</v>
-      </c>
-      <c r="R15" s="8">
-        <v>0</v>
-      </c>
-      <c r="S15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8">
+        <v>3</v>
+      </c>
+      <c r="H17" s="8">
+        <v>3</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="9"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75">
+      <c r="A18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="8">
+        <v>20</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8">
+        <v>4</v>
+      </c>
+      <c r="G18" s="8">
+        <v>4</v>
+      </c>
+      <c r="H18" s="8">
+        <v>4</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="9"/>
+    </row>
+    <row r="19" spans="1:19" ht="15.75">
+      <c r="A19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="8">
+        <v>20</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8">
+        <v>4</v>
+      </c>
+      <c r="G19" s="8">
+        <v>4</v>
+      </c>
+      <c r="H19" s="8">
+        <v>4</v>
+      </c>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="9"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75">
+      <c r="A20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="22" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="14">
-        <f>SUM(D2:D15)</f>
-        <v>124</v>
-      </c>
-      <c r="E16" s="15">
-        <f t="shared" ref="E16:R16" si="0">(F16-$S$16/14)</f>
-        <v>-4.2632564145606011E-14</v>
-      </c>
-      <c r="F16" s="15">
-        <f t="shared" si="0"/>
-        <v>8.857142857142815</v>
-      </c>
-      <c r="G16" s="15">
-        <f t="shared" si="0"/>
-        <v>17.714285714285673</v>
-      </c>
-      <c r="H16" s="15">
-        <f>(I16-$S$16/14)</f>
-        <v>26.57142857142853</v>
-      </c>
-      <c r="I16" s="15">
-        <f t="shared" si="0"/>
-        <v>35.428571428571388</v>
-      </c>
-      <c r="J16" s="15">
-        <f t="shared" si="0"/>
-        <v>44.285714285714249</v>
-      </c>
-      <c r="K16" s="15">
-        <f t="shared" si="0"/>
-        <v>53.14285714285711</v>
-      </c>
-      <c r="L16" s="15">
-        <f t="shared" si="0"/>
-        <v>61.999999999999972</v>
-      </c>
-      <c r="M16" s="15">
-        <f t="shared" si="0"/>
-        <v>70.857142857142833</v>
-      </c>
-      <c r="N16" s="15">
-        <f t="shared" si="0"/>
-        <v>79.714285714285694</v>
-      </c>
-      <c r="O16" s="15">
-        <f t="shared" si="0"/>
-        <v>88.571428571428555</v>
-      </c>
-      <c r="P16" s="15">
-        <f t="shared" si="0"/>
-        <v>97.428571428571416</v>
-      </c>
-      <c r="Q16" s="15">
-        <f t="shared" si="0"/>
-        <v>106.28571428571428</v>
-      </c>
-      <c r="R16" s="15">
-        <f t="shared" si="0"/>
-        <v>115.14285714285714</v>
-      </c>
-      <c r="S16" s="16">
-        <f>SUM(D2:D15)</f>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="D20" s="14">
+        <f>SUM(D2:D19)</f>
+        <v>164</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0</v>
+      </c>
+      <c r="F20" s="15">
+        <f>(H20-$D$20/6)</f>
+        <v>36.444444444444443</v>
+      </c>
+      <c r="G20" s="15">
+        <f>(F20)</f>
+        <v>36.444444444444443</v>
+      </c>
+      <c r="H20" s="15">
+        <f>(J20-$M$20/6)</f>
+        <v>63.777777777777779</v>
+      </c>
+      <c r="I20" s="15">
+        <f>(H20)</f>
+        <v>63.777777777777779</v>
+      </c>
+      <c r="J20" s="15">
+        <f>(M20-$D$20/6)</f>
+        <v>82</v>
+      </c>
+      <c r="K20" s="15">
+        <f>(J20)</f>
+        <v>82</v>
+      </c>
+      <c r="L20" s="15">
+        <f>(J20)</f>
+        <v>82</v>
+      </c>
+      <c r="M20" s="15">
+        <f>(O20-$D$20/6)</f>
+        <v>109.33333333333333</v>
+      </c>
+      <c r="N20" s="15">
+        <f>(M20)</f>
+        <v>109.33333333333333</v>
+      </c>
+      <c r="O20" s="15">
+        <f>(Q20-$D$20/6)</f>
+        <v>136.66666666666666</v>
+      </c>
+      <c r="P20" s="15">
+        <f>(O20)</f>
+        <v>136.66666666666666</v>
+      </c>
+      <c r="Q20" s="15">
+        <f>(D20)</f>
+        <v>164</v>
+      </c>
+      <c r="R20" s="15">
+        <f>(Q20)</f>
+        <v>164</v>
+      </c>
+      <c r="S20" s="16">
+        <f>(Q20)</f>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="15.75">
+      <c r="A21" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19">
-        <f t="shared" ref="E17:S17" si="1">SUM(E1:E15)</f>
-        <v>6.5</v>
-      </c>
-      <c r="F17" s="19">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="G17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S17" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19">
+        <f>SUM(E1:E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="19">
+        <f>SUM(F1:F19)</f>
+        <v>22</v>
+      </c>
+      <c r="G21" s="19">
+        <f>SUM(G1:G19)</f>
+        <v>22</v>
+      </c>
+      <c r="H21" s="19">
+        <f>SUM(H1:H19)</f>
+        <v>22</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="25"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.75">
+      <c r="A22" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B22" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="2"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2122,24 +1859,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>